<commit_message>
TFS 11259 - Add users to production DB
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C40275
</commit_message>
<xml_diff>
--- a/Project Management/CCO_eCoaching_Log_Permissions.xlsx
+++ b/Project Management/CCO_eCoaching_Log_Permissions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21840" windowHeight="13740" tabRatio="931" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21840" windowHeight="13740" tabRatio="931"/>
   </bookViews>
   <sheets>
     <sheet name="Revisions History" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5069" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5107" uniqueCount="459">
   <si>
     <t>name</t>
   </si>
@@ -1751,21 +1751,12 @@
     <t>\\F3420-ECLDBP01\ETS\</t>
   </si>
   <si>
-    <t>AD\Nicole.Fry, AD\Derel.Bennett, AD\Cheryl.Fiala, AD\Camesha.Hampton, AD\Michaela.Roberts, AD\Linsay.Hartman</t>
-  </si>
-  <si>
     <t>\\F3420-ECLDBP01\Generic\</t>
   </si>
   <si>
-    <t>AD\Jennifer.Foster, AD\Susan.Rager</t>
-  </si>
-  <si>
     <t>\\F3420-ECLDBP01\IQS\</t>
   </si>
   <si>
-    <t>VNGT\QMTasks</t>
-  </si>
-  <si>
     <t>\\F3420-ECLDBP01\Outliers\</t>
   </si>
   <si>
@@ -1775,9 +1766,6 @@
     <t>\\F3420-ECLDBP01\Quality\</t>
   </si>
   <si>
-    <t>AD\Scott.Potter, AD\Jennifer.Foster, AD\Tyler.McQuillan, AD\Jeffery.Ross, AD\Christopher.Gary</t>
-  </si>
-  <si>
     <t>\\F3420-ECLDBP01\Reports\</t>
   </si>
   <si>
@@ -1788,9 +1776,6 @@
   </si>
   <si>
     <t>AD\Daniel.Callahan, AD\Jacqueline.McCutcheon, AD\Mandy.Pratt</t>
-  </si>
-  <si>
-    <t>VNGT\aspectuser, VNGT\QMTask, SVC-F1220-PSFT,VNGT\svc-appeasesqlt01,AD\SA-Lex.Mishra,AD\lex.mishra</t>
   </si>
   <si>
     <t>H:\Data\Coaching\HrInfo\</t>
@@ -1845,6 +1830,63 @@
 AD\sa-susmitha.Palacher
 AD\sa-david.hinman
 AD\sa-lili.huang</t>
+  </si>
+  <si>
+    <t>10.0</t>
+  </si>
+  <si>
+    <t>Requested by tim Queen. Approved by Mike Ingram. IR2838924</t>
+  </si>
+  <si>
+    <t>AD\John.Sweeney</t>
+  </si>
+  <si>
+    <t>AD\Kyle.Munz</t>
+  </si>
+  <si>
+    <t>AD\Chelsie.Norris</t>
+  </si>
+  <si>
+    <t>AD\Sara.Stonecipher</t>
+  </si>
+  <si>
+    <t>AD\Shelly.Encke</t>
+  </si>
+  <si>
+    <t>H:\Data\</t>
+  </si>
+  <si>
+    <t>I:\Data\</t>
+  </si>
+  <si>
+    <t>VNGT\aspectuser, SVC-F1220-PSFT,VNGT\svc-appeasesqlt01,AD\SA-Lex.Mishra,AD\lex.mishra</t>
+  </si>
+  <si>
+    <t>AD\Nicole.Fry, AD\Derek.Bennett, AD\Cheryl.Fiala, AD\Camesha.Hampton, AD\Michaela.Roberts, AD\Lindsay.Hartman</t>
+  </si>
+  <si>
+    <t>AD\Jennifer.Foster, AD\Susan.Rager,AD\scott.potter</t>
+  </si>
+  <si>
+    <t>AD\Scott.Potter, AD\Jennifer.Foster, AD\Tyler.McQuillan, AD\Jeffery.Ross, AD\Christopher.Gray</t>
+  </si>
+  <si>
+    <t>\\f3420-ecldbd01\data\Coaching\IQS\</t>
+  </si>
+  <si>
+    <t>AD\SVC-F3420-APPIQST01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">READ/WRITE/LIST CONTENTS/MODIFY </t>
+  </si>
+  <si>
+    <t>\\f3420-ecldbt01\data\Coaching\IQS\</t>
+  </si>
+  <si>
+    <t>AD\SVC-F3420-APPIQSP01,AD\Lola.Treinen</t>
+  </si>
+  <si>
+    <t>TFS 11259 - Add query access for users to production database (database access tab)</t>
   </si>
 </sst>
 </file>
@@ -2144,7 +2186,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2220,6 +2262,13 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2234,6 +2283,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2266,9 +2318,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2550,10 +2604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2740,6 +2794,23 @@
       </c>
       <c r="E12" t="s">
         <v>396</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="65">
+        <v>43262</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>440</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>458</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" t="s">
+        <v>441</v>
       </c>
     </row>
   </sheetData>
@@ -4938,10 +5009,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="52" t="s">
         <v>129</v>
       </c>
-      <c r="B2" s="46"/>
+      <c r="B2" s="49"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
@@ -4953,11 +5024,11 @@
       <c r="C4" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="D4" s="49" t="s">
+      <c r="D4" s="53" t="s">
         <v>108</v>
       </c>
-      <c r="E4" s="50"/>
-      <c r="F4" s="51"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="55"/>
       <c r="G4" s="20" t="s">
         <v>109</v>
       </c>
@@ -4972,23 +5043,23 @@
       <c r="C5" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="D5" s="52" t="s">
+      <c r="D5" s="56" t="s">
         <v>126</v>
       </c>
-      <c r="E5" s="53"/>
-      <c r="F5" s="54"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="58"/>
       <c r="G5" s="24" t="s">
         <v>104</v>
       </c>
       <c r="H5" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="I5" s="55" t="s">
+      <c r="I5" s="59" t="s">
         <v>112</v>
       </c>
-      <c r="J5" s="55"/>
-      <c r="K5" s="55"/>
-      <c r="L5" s="55"/>
+      <c r="J5" s="59"/>
+      <c r="K5" s="59"/>
+      <c r="L5" s="59"/>
     </row>
     <row r="6" spans="1:12" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
@@ -5000,11 +5071,11 @@
       <c r="C6" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="D6" s="52" t="s">
+      <c r="D6" s="56" t="s">
         <v>116</v>
       </c>
-      <c r="E6" s="53"/>
-      <c r="F6" s="54"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="58"/>
       <c r="G6" s="21" t="s">
         <v>104</v>
       </c>
@@ -5019,11 +5090,11 @@
       <c r="C7" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="D7" s="56" t="s">
+      <c r="D7" s="60" t="s">
         <v>120</v>
       </c>
-      <c r="E7" s="57"/>
-      <c r="F7" s="58"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="62"/>
       <c r="G7" s="24" t="s">
         <v>104</v>
       </c>
@@ -5032,10 +5103,10 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="59" t="s">
+      <c r="A10" s="52" t="s">
         <v>128</v>
       </c>
-      <c r="B10" s="46"/>
+      <c r="B10" s="49"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
@@ -5047,11 +5118,11 @@
       <c r="C12" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="D12" s="49" t="s">
+      <c r="D12" s="53" t="s">
         <v>108</v>
       </c>
-      <c r="E12" s="50"/>
-      <c r="F12" s="51"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="55"/>
       <c r="G12" s="20" t="s">
         <v>109</v>
       </c>
@@ -5066,23 +5137,23 @@
       <c r="C13" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="D13" s="52" t="s">
+      <c r="D13" s="56" t="s">
         <v>127</v>
       </c>
-      <c r="E13" s="53"/>
-      <c r="F13" s="54"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="58"/>
       <c r="G13" s="24" t="s">
         <v>104</v>
       </c>
       <c r="H13" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="I13" s="55" t="s">
+      <c r="I13" s="59" t="s">
         <v>112</v>
       </c>
-      <c r="J13" s="55"/>
-      <c r="K13" s="55"/>
-      <c r="L13" s="55"/>
+      <c r="J13" s="59"/>
+      <c r="K13" s="59"/>
+      <c r="L13" s="59"/>
     </row>
     <row r="14" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
@@ -5094,11 +5165,11 @@
       <c r="C14" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="D14" s="52" t="s">
+      <c r="D14" s="56" t="s">
         <v>123</v>
       </c>
-      <c r="E14" s="53"/>
-      <c r="F14" s="54"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="58"/>
       <c r="G14" s="21" t="s">
         <v>104</v>
       </c>
@@ -5113,11 +5184,11 @@
       <c r="C15" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="D15" s="56" t="s">
+      <c r="D15" s="60" t="s">
         <v>125</v>
       </c>
-      <c r="E15" s="57"/>
-      <c r="F15" s="58"/>
+      <c r="E15" s="61"/>
+      <c r="F15" s="62"/>
       <c r="G15" s="24" t="s">
         <v>104</v>
       </c>
@@ -5127,6 +5198,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="I13:L13"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D15:F15"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="D4:F4"/>
@@ -5134,11 +5210,6 @@
     <mergeCell ref="I5:L5"/>
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="I13:L13"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D15:F15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
@@ -13016,7 +13087,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="A31" sqref="A31:A33"/>
     </sheetView>
   </sheetViews>
@@ -13419,10 +13490,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13899,6 +13970,97 @@
       <c r="I28" t="s">
         <v>41</v>
       </c>
+      <c r="J28" s="43" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="63" t="s">
+        <v>442</v>
+      </c>
+      <c r="B29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" t="s">
+        <v>402</v>
+      </c>
+      <c r="I29" t="s">
+        <v>41</v>
+      </c>
+      <c r="J29" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="63" t="s">
+        <v>443</v>
+      </c>
+      <c r="B30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" t="s">
+        <v>402</v>
+      </c>
+      <c r="I30" t="s">
+        <v>41</v>
+      </c>
+      <c r="J30" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="63" t="s">
+        <v>444</v>
+      </c>
+      <c r="B31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
+        <v>402</v>
+      </c>
+      <c r="I31" t="s">
+        <v>41</v>
+      </c>
+      <c r="J31" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A32" s="63" t="s">
+        <v>445</v>
+      </c>
+      <c r="B32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>402</v>
+      </c>
+      <c r="F32" t="s">
+        <v>41</v>
+      </c>
+      <c r="J32" s="43" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A33" s="63" t="s">
+        <v>446</v>
+      </c>
+      <c r="B33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" t="s">
+        <v>402</v>
+      </c>
+      <c r="F33" t="s">
+        <v>41</v>
+      </c>
+      <c r="J33" s="43" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J34"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I1">
@@ -13913,10 +14075,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:A36"/>
+    <sheetView topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13932,13 +14094,13 @@
       <c r="A1" s="14" t="s">
         <v>403</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="46" t="s">
         <v>169</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>403</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="46" t="s">
         <v>412</v>
       </c>
     </row>
@@ -13946,11 +14108,11 @@
       <c r="A2" s="16" t="s">
         <v>404</v>
       </c>
-      <c r="B2" s="44"/>
+      <c r="B2" s="47"/>
       <c r="D2" s="16" t="s">
         <v>410</v>
       </c>
-      <c r="E2" s="44"/>
+      <c r="E2" s="47"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
@@ -13967,511 +14129,585 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="48" t="s">
         <v>406</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="D5" s="45" t="s">
+      <c r="D5" s="48" t="s">
         <v>406</v>
       </c>
-      <c r="E5" s="45" t="s">
+      <c r="E5" s="48" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="46"/>
-      <c r="B6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
+      <c r="A6" s="49"/>
+      <c r="B6" s="49"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="46"/>
-      <c r="B7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
+      <c r="A7" s="49"/>
+      <c r="B7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="46"/>
-      <c r="B8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
+      <c r="A8" s="49"/>
+      <c r="B8" s="49"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="46"/>
-      <c r="B9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
+      <c r="A9" s="49"/>
+      <c r="B9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="46"/>
-      <c r="B10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
+      <c r="A10" s="49"/>
+      <c r="B10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="46"/>
-      <c r="B11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
+      <c r="A11" s="49"/>
+      <c r="B11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="46"/>
-      <c r="B12" s="46"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
+      <c r="A12" s="49"/>
+      <c r="B12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="46"/>
-      <c r="B13" s="46"/>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
+      <c r="A13" s="49"/>
+      <c r="B13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="46"/>
-      <c r="B14" s="46"/>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46"/>
+      <c r="A14" s="49"/>
+      <c r="B14" s="49"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="46"/>
-      <c r="B15" s="46"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="46"/>
+      <c r="A15" s="49"/>
+      <c r="B15" s="49"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="46"/>
-      <c r="B16" s="46"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
+      <c r="A16" s="49"/>
+      <c r="B16" s="49"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="46"/>
-      <c r="B17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
+      <c r="A17" s="49"/>
+      <c r="B17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="34"/>
-      <c r="B18" s="34"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="34"/>
-      <c r="B19" s="34"/>
+      <c r="A18" s="44"/>
+      <c r="B18" s="44"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="44"/>
+    </row>
+    <row r="19" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="44"/>
+      <c r="D19" s="45" t="s">
+        <v>453</v>
+      </c>
+      <c r="E19" s="49" t="s">
+        <v>455</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="44"/>
+      <c r="D20" t="s">
+        <v>454</v>
+      </c>
+      <c r="E20" s="49"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="44"/>
+      <c r="B21" s="44"/>
+      <c r="D21" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="44"/>
+      <c r="B22" s="44"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="34"/>
+      <c r="B23" s="44"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="14" t="s">
         <v>407</v>
       </c>
-      <c r="B20" s="43" t="s">
+      <c r="B24" s="34"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="16" t="s">
+        <v>409</v>
+      </c>
+      <c r="B25" s="46" t="s">
         <v>169</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D25" s="14" t="s">
         <v>407</v>
       </c>
-      <c r="E20" s="43" t="s">
+      <c r="E25" s="46" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="16" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="16" t="s">
+        <v>408</v>
+      </c>
+      <c r="B26" s="47"/>
+      <c r="D26" s="16" t="s">
         <v>409</v>
       </c>
-      <c r="B21" s="44"/>
-      <c r="D21" s="16" t="s">
-        <v>409</v>
-      </c>
-      <c r="E21" s="44"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="16" t="s">
-        <v>408</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="E26" s="47"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
         <v>365</v>
       </c>
-      <c r="D22" s="16" t="s">
-        <v>408</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="D27" s="16" t="s">
+        <v>448</v>
+      </c>
+      <c r="E27" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="45" t="s">
-        <v>443</v>
-      </c>
-      <c r="B24" s="45" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="48" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="49"/>
+      <c r="B29" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="D24" s="45" t="s">
-        <v>443</v>
-      </c>
-      <c r="E24" s="45" t="s">
+      <c r="D29" s="48" t="s">
+        <v>438</v>
+      </c>
+      <c r="E29" s="48" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="46"/>
-      <c r="B25" s="46"/>
-      <c r="D25" s="46"/>
-      <c r="E25" s="46"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="46"/>
-      <c r="B26" s="46"/>
-      <c r="D26" s="46"/>
-      <c r="E26" s="46"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="46"/>
-      <c r="B27" s="46"/>
-      <c r="D27" s="46"/>
-      <c r="E27" s="46"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="46"/>
-      <c r="B28" s="46"/>
-      <c r="D28" s="46"/>
-      <c r="E28" s="46"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="46"/>
-      <c r="B29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="46"/>
-      <c r="B30" s="46"/>
-      <c r="D30" s="46"/>
-      <c r="E30" s="46"/>
+    <row r="30" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="49"/>
+      <c r="B30" s="49"/>
+      <c r="D30" s="49"/>
+      <c r="E30" s="49"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="46"/>
-      <c r="B31" s="46"/>
-      <c r="D31" s="46"/>
-      <c r="E31" s="46"/>
+      <c r="A31" s="49"/>
+      <c r="B31" s="49"/>
+      <c r="D31" s="49"/>
+      <c r="E31" s="49"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="46"/>
-      <c r="B32" s="46"/>
-      <c r="D32" s="46"/>
-      <c r="E32" s="46"/>
+      <c r="A32" s="49"/>
+      <c r="B32" s="49"/>
+      <c r="D32" s="49"/>
+      <c r="E32" s="49"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="46"/>
-      <c r="B33" s="46"/>
-      <c r="D33" s="46"/>
-      <c r="E33" s="46"/>
+      <c r="A33" s="49"/>
+      <c r="B33" s="49"/>
+      <c r="D33" s="49"/>
+      <c r="E33" s="49"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="46"/>
-      <c r="B34" s="46"/>
-      <c r="D34" s="46"/>
-      <c r="E34" s="46"/>
+      <c r="A34" s="49"/>
+      <c r="B34" s="49"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="49"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="46"/>
-      <c r="B35" s="46"/>
-      <c r="D35" s="46"/>
-      <c r="E35" s="46"/>
+      <c r="A35" s="49"/>
+      <c r="B35" s="49"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="49"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="46"/>
-      <c r="B36" s="46"/>
-      <c r="D36" s="46"/>
-      <c r="E36" s="46"/>
+      <c r="A36" s="49"/>
+      <c r="B36" s="49"/>
+      <c r="D36" s="49"/>
+      <c r="E36" s="49"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="49"/>
+      <c r="B37" s="49"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="49"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="49"/>
+      <c r="B38" s="49"/>
+      <c r="D38" s="49"/>
+      <c r="E38" s="49"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="49"/>
+      <c r="B39" s="49"/>
+      <c r="D39" s="49"/>
+      <c r="E39" s="49"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="14" t="s">
+      <c r="A40" s="49"/>
+      <c r="B40" s="49"/>
+      <c r="D40" s="49"/>
+      <c r="E40" s="49"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B41" s="49"/>
+      <c r="D41" s="49"/>
+      <c r="E41" s="49"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="44"/>
+      <c r="B42" s="44"/>
+      <c r="D42" s="44"/>
+      <c r="E42" s="44"/>
+    </row>
+    <row r="43" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A43" s="44"/>
+      <c r="D43" s="64" t="s">
+        <v>456</v>
+      </c>
+      <c r="E43" s="49" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="44"/>
+      <c r="D44" t="s">
+        <v>454</v>
+      </c>
+      <c r="E44" s="49"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="44"/>
+      <c r="B45" s="44"/>
+      <c r="D45" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="44"/>
+      <c r="B46" s="44"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="14" t="s">
         <v>413</v>
       </c>
-      <c r="B40" s="43" t="s">
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="16" t="s">
+        <v>414</v>
+      </c>
+      <c r="B50" s="46" t="s">
         <v>169</v>
       </c>
-      <c r="D40" s="14" t="s">
+      <c r="D50" s="14" t="s">
         <v>413</v>
       </c>
-      <c r="E40" s="43" t="s">
+      <c r="E50" s="46" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="16" t="s">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="16" t="s">
+        <v>415</v>
+      </c>
+      <c r="B51" s="47"/>
+      <c r="D51" s="16" t="s">
         <v>414</v>
       </c>
-      <c r="B41" s="44"/>
-      <c r="D41" s="16" t="s">
-        <v>414</v>
-      </c>
-      <c r="E41" s="44"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="16" t="s">
-        <v>415</v>
-      </c>
-      <c r="B42" t="s">
+      <c r="E51" s="47"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
         <v>365</v>
       </c>
-      <c r="D42" s="16" t="s">
-        <v>415</v>
-      </c>
-      <c r="E42" t="s">
+      <c r="D52" s="16" t="s">
+        <v>447</v>
+      </c>
+      <c r="E52" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="45" t="s">
-        <v>444</v>
-      </c>
-      <c r="B44" s="45" t="s">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="48" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="49"/>
+      <c r="B54" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="D44" s="45" t="s">
-        <v>444</v>
-      </c>
-      <c r="E44" s="45" t="s">
+      <c r="D54" s="48" t="s">
+        <v>439</v>
+      </c>
+      <c r="E54" s="48" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="46"/>
-      <c r="B45" s="46"/>
-      <c r="D45" s="46"/>
-      <c r="E45" s="46"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="46"/>
-      <c r="B46" s="46"/>
-      <c r="D46" s="46"/>
-      <c r="E46" s="46"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="46"/>
-      <c r="B47" s="46"/>
-      <c r="D47" s="46"/>
-      <c r="E47" s="46"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="46"/>
-      <c r="B48" s="46"/>
-      <c r="D48" s="46"/>
-      <c r="E48" s="46"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="46"/>
-      <c r="B49" s="46"/>
-      <c r="D49" s="46"/>
-      <c r="E49" s="46"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="46"/>
-      <c r="B50" s="46"/>
-      <c r="D50" s="46"/>
-      <c r="E50" s="46"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="46"/>
-      <c r="B51" s="46"/>
-      <c r="D51" s="46"/>
-      <c r="E51" s="46"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" s="46"/>
-      <c r="B52" s="46"/>
-      <c r="D52" s="46"/>
-      <c r="E52" s="46"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" s="46"/>
-      <c r="B53" s="46"/>
-      <c r="D53" s="46"/>
-      <c r="E53" s="46"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" s="46"/>
-      <c r="B54" s="46"/>
-      <c r="D54" s="46"/>
-      <c r="E54" s="46"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" s="46"/>
-      <c r="B55" s="46"/>
-      <c r="D55" s="46"/>
-      <c r="E55" s="46"/>
+    <row r="55" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="49"/>
+      <c r="B55" s="49"/>
+      <c r="D55" s="49"/>
+      <c r="E55" s="49"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" s="46"/>
-      <c r="B56" s="46"/>
-      <c r="D56" s="46"/>
-      <c r="E56" s="46"/>
+      <c r="A56" s="49"/>
+      <c r="B56" s="49"/>
+      <c r="D56" s="49"/>
+      <c r="E56" s="49"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" s="49"/>
+      <c r="B57" s="49"/>
+      <c r="D57" s="49"/>
+      <c r="E57" s="49"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" s="49"/>
+      <c r="B58" s="49"/>
+      <c r="D58" s="49"/>
+      <c r="E58" s="49"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" s="14" t="s">
+      <c r="A59" s="49"/>
+      <c r="B59" s="49"/>
+      <c r="D59" s="49"/>
+      <c r="E59" s="49"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" s="49"/>
+      <c r="B60" s="49"/>
+      <c r="D60" s="49"/>
+      <c r="E60" s="49"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" s="49"/>
+      <c r="B61" s="49"/>
+      <c r="D61" s="49"/>
+      <c r="E61" s="49"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" s="49"/>
+      <c r="B62" s="49"/>
+      <c r="D62" s="49"/>
+      <c r="E62" s="49"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" s="49"/>
+      <c r="B63" s="49"/>
+      <c r="D63" s="49"/>
+      <c r="E63" s="49"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" s="49"/>
+      <c r="B64" s="49"/>
+      <c r="D64" s="49"/>
+      <c r="E64" s="49"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" s="49"/>
+      <c r="B65" s="49"/>
+      <c r="D65" s="49"/>
+      <c r="E65" s="49"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B66" s="49"/>
+      <c r="D66" s="49"/>
+      <c r="E66" s="49"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69" s="14" t="s">
         <v>416</v>
       </c>
-      <c r="B59" s="14" t="s">
+      <c r="B69" s="14" t="s">
         <v>417</v>
       </c>
-      <c r="C59" s="14" t="s">
+      <c r="C69" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="D59" s="14" t="s">
+      <c r="D69" s="14" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" s="37" t="s">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" s="37" t="s">
+        <v>430</v>
+      </c>
+      <c r="B70" s="38" t="s">
+        <v>418</v>
+      </c>
+      <c r="C70" s="39" t="s">
+        <v>449</v>
+      </c>
+      <c r="D70" s="37" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="40" t="s">
+        <v>431</v>
+      </c>
+      <c r="B71" s="41" t="s">
+        <v>420</v>
+      </c>
+      <c r="C71" s="42" t="s">
+        <v>450</v>
+      </c>
+      <c r="D71" s="40" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="37" t="s">
+        <v>432</v>
+      </c>
+      <c r="B72" s="38" t="s">
+        <v>421</v>
+      </c>
+      <c r="C72" s="39" t="s">
+        <v>451</v>
+      </c>
+      <c r="D72" s="37" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73" s="40" t="s">
+        <v>433</v>
+      </c>
+      <c r="B73" s="41" t="s">
+        <v>422</v>
+      </c>
+      <c r="C73" s="42" t="s">
+        <v>457</v>
+      </c>
+      <c r="D73" s="40" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74" s="37" t="s">
+        <v>434</v>
+      </c>
+      <c r="B74" s="38" t="s">
+        <v>423</v>
+      </c>
+      <c r="C74" s="39" t="s">
+        <v>424</v>
+      </c>
+      <c r="D74" s="37" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75" s="40" t="s">
         <v>435</v>
       </c>
-      <c r="B60" s="38" t="s">
-        <v>418</v>
-      </c>
-      <c r="C60" s="39" t="s">
-        <v>434</v>
-      </c>
-      <c r="D60" s="37" t="s">
+      <c r="B75" s="41" t="s">
+        <v>425</v>
+      </c>
+      <c r="C75" s="42" t="s">
+        <v>452</v>
+      </c>
+      <c r="D75" s="40" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="40" t="s">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76" s="37" t="s">
         <v>436</v>
       </c>
-      <c r="B61" s="41" t="s">
-        <v>420</v>
-      </c>
-      <c r="C61" s="42" t="s">
-        <v>421</v>
-      </c>
-      <c r="D61" s="40" t="s">
+      <c r="B76" s="38" t="s">
+        <v>426</v>
+      </c>
+      <c r="C76" s="39" t="s">
+        <v>427</v>
+      </c>
+      <c r="D76" s="37" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="37" t="s">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77" s="37" t="s">
         <v>437</v>
       </c>
-      <c r="B62" s="38" t="s">
-        <v>422</v>
-      </c>
-      <c r="C62" s="39" t="s">
-        <v>423</v>
-      </c>
-      <c r="D62" s="37" t="s">
+      <c r="B77" s="38" t="s">
+        <v>428</v>
+      </c>
+      <c r="C77" s="39" t="s">
+        <v>429</v>
+      </c>
+      <c r="D77" s="37" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A63" s="40" t="s">
-        <v>438</v>
-      </c>
-      <c r="B63" s="41" t="s">
-        <v>424</v>
-      </c>
-      <c r="C63" s="42" t="s">
-        <v>425</v>
-      </c>
-      <c r="D63" s="40" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A64" s="37" t="s">
-        <v>439</v>
-      </c>
-      <c r="B64" s="38" t="s">
-        <v>426</v>
-      </c>
-      <c r="C64" s="39" t="s">
-        <v>427</v>
-      </c>
-      <c r="D64" s="37" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="40" t="s">
-        <v>440</v>
-      </c>
-      <c r="B65" s="41" t="s">
-        <v>428</v>
-      </c>
-      <c r="C65" s="42" t="s">
-        <v>429</v>
-      </c>
-      <c r="D65" s="40" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="37" t="s">
-        <v>441</v>
-      </c>
-      <c r="B66" s="38" t="s">
-        <v>430</v>
-      </c>
-      <c r="C66" s="39" t="s">
-        <v>431</v>
-      </c>
-      <c r="D66" s="37" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="37" t="s">
-        <v>442</v>
-      </c>
-      <c r="B67" s="38" t="s">
-        <v>432</v>
-      </c>
-      <c r="C67" s="39" t="s">
-        <v>433</v>
-      </c>
-      <c r="D67" s="37" t="s">
-        <v>419</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="20">
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="A53:A65"/>
+    <mergeCell ref="B54:B66"/>
+    <mergeCell ref="D54:D66"/>
+    <mergeCell ref="E54:E66"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D5:D17"/>
+    <mergeCell ref="E5:E17"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="D29:D41"/>
+    <mergeCell ref="E29:E41"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A5:A17"/>
     <mergeCell ref="B5:B17"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A24:A36"/>
-    <mergeCell ref="B24:B36"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D5:D17"/>
-    <mergeCell ref="E5:E17"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="D24:D36"/>
-    <mergeCell ref="E24:E36"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="A44:A56"/>
-    <mergeCell ref="B44:B56"/>
-    <mergeCell ref="D44:D56"/>
-    <mergeCell ref="E44:E56"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="A28:A40"/>
+    <mergeCell ref="B29:B41"/>
+    <mergeCell ref="E19:E20"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A21" r:id="rId1"/>
+    <hyperlink ref="A25" r:id="rId1"/>
     <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="D21" r:id="rId3"/>
-    <hyperlink ref="A41" r:id="rId4"/>
-    <hyperlink ref="D41" r:id="rId5"/>
-    <hyperlink ref="B60" r:id="rId6"/>
-    <hyperlink ref="B61" r:id="rId7"/>
-    <hyperlink ref="B62" r:id="rId8"/>
-    <hyperlink ref="B63" r:id="rId9"/>
-    <hyperlink ref="B64" r:id="rId10"/>
-    <hyperlink ref="B65" r:id="rId11"/>
-    <hyperlink ref="B66" r:id="rId12"/>
-    <hyperlink ref="B67" r:id="rId13"/>
+    <hyperlink ref="D26" r:id="rId3"/>
+    <hyperlink ref="A50" r:id="rId4"/>
+    <hyperlink ref="D51" r:id="rId5"/>
+    <hyperlink ref="B70" r:id="rId6"/>
+    <hyperlink ref="B71" r:id="rId7"/>
+    <hyperlink ref="B72" r:id="rId8"/>
+    <hyperlink ref="B73" r:id="rId9"/>
+    <hyperlink ref="B74" r:id="rId10"/>
+    <hyperlink ref="B75" r:id="rId11"/>
+    <hyperlink ref="B76" r:id="rId12"/>
+    <hyperlink ref="B77" r:id="rId13"/>
+    <hyperlink ref="D43" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId14"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
 
@@ -14494,7 +14730,7 @@
       <c r="A1" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="46" t="s">
         <v>171</v>
       </c>
     </row>
@@ -14502,7 +14738,7 @@
       <c r="A2" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="B2" s="44"/>
+      <c r="B2" s="47"/>
       <c r="C2" s="27"/>
       <c r="D2" s="27"/>
       <c r="E2" s="27"/>
@@ -14981,7 +15217,7 @@
       <c r="B81" t="s">
         <v>101</v>
       </c>
-      <c r="C81" s="45" t="s">
+      <c r="C81" s="48" t="s">
         <v>103</v>
       </c>
     </row>
@@ -14992,31 +15228,31 @@
       <c r="B82" t="s">
         <v>102</v>
       </c>
-      <c r="C82" s="45"/>
+      <c r="C82" s="48"/>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B83" t="s">
         <v>131</v>
       </c>
-      <c r="C83" s="45"/>
+      <c r="C83" s="48"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B84" t="s">
         <v>132</v>
       </c>
-      <c r="C84" s="45"/>
+      <c r="C84" s="48"/>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B85" t="s">
         <v>100</v>
       </c>
-      <c r="C85" s="45"/>
+      <c r="C85" s="48"/>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B86" t="s">
         <v>101</v>
       </c>
-      <c r="C86" s="45"/>
+      <c r="C86" s="48"/>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
@@ -15025,7 +15261,7 @@
       <c r="B87" t="s">
         <v>99</v>
       </c>
-      <c r="C87" s="45"/>
+      <c r="C87" s="48"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
@@ -15034,7 +15270,7 @@
       <c r="B88" t="s">
         <v>131</v>
       </c>
-      <c r="C88" s="45"/>
+      <c r="C88" s="48"/>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B89" t="s">
@@ -15117,7 +15353,7 @@
       <c r="A102" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="B102" s="43" t="s">
+      <c r="B102" s="46" t="s">
         <v>170</v>
       </c>
     </row>
@@ -15125,7 +15361,7 @@
       <c r="A103" s="28" t="s">
         <v>168</v>
       </c>
-      <c r="B103" s="44"/>
+      <c r="B103" s="47"/>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
@@ -15466,7 +15702,7 @@
       <c r="B160" t="s">
         <v>102</v>
       </c>
-      <c r="C160" s="45" t="s">
+      <c r="C160" s="48" t="s">
         <v>103</v>
       </c>
     </row>
@@ -15474,25 +15710,25 @@
       <c r="B161" t="s">
         <v>131</v>
       </c>
-      <c r="C161" s="45"/>
+      <c r="C161" s="48"/>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B162" t="s">
         <v>132</v>
       </c>
-      <c r="C162" s="45"/>
+      <c r="C162" s="48"/>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B163" t="s">
         <v>100</v>
       </c>
-      <c r="C163" s="45"/>
+      <c r="C163" s="48"/>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B164" t="s">
         <v>101</v>
       </c>
-      <c r="C164" s="45"/>
+      <c r="C164" s="48"/>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
@@ -15501,7 +15737,7 @@
       <c r="B165" t="s">
         <v>99</v>
       </c>
-      <c r="C165" s="45"/>
+      <c r="C165" s="48"/>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
@@ -15510,13 +15746,13 @@
       <c r="B166" t="s">
         <v>102</v>
       </c>
-      <c r="C166" s="45"/>
+      <c r="C166" s="48"/>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B167" t="s">
         <v>131</v>
       </c>
-      <c r="C167" s="45"/>
+      <c r="C167" s="48"/>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B168" t="s">
@@ -16632,10 +16868,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="50" t="s">
         <v>189</v>
       </c>
-      <c r="B1" s="48"/>
+      <c r="B1" s="51"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">

</xml_diff>